<commit_message>
Add uart program guide .xml sheet
</commit_message>
<xml_diff>
--- a/docs/UART_reference.xlsx
+++ b/docs/UART_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,8 @@
     <sheet name="IPDESCR_rel1.0.0" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="IPREGLIST_rel1.0.0" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="IPREGMAP_rel1.0.0" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="VerPlan_rel1.0.0" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="IP_Porgram_Guide_rel1.0.0" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="VerPlan_rel1.0.0" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="IF_DIR" vbProcedure="false">#REF!</definedName>
@@ -25,9 +26,9 @@
     <definedName function="false" hidden="false" name="IF_TYPE" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="IF_VOLTAGE" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="REGISTERTYPE_LIST" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="IF_DIR" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="IF_IO" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="IF_ISO" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="IF_DIR" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="IF_IO" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="IF_ISO" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,69 +40,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="220">
-  <si>
-    <t>Document Information</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>UART reference</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>IP reference</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Florent Rotenberg</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Fisrt Release</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>UART interface definition</t>
-  </si>
-  <si>
-    <t>IP Information</t>
-  </si>
-  <si>
-    <t>IP type</t>
-  </si>
-  <si>
-    <t>UART</t>
-  </si>
-  <si>
-    <t>Delivery Type</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Modification</t>
-  </si>
-  <si>
-    <t>26/10/2016</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="256">
+  <si>
+    <t xml:space="preserve">Document Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florent Rotenberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fisrt Release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART interface definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/10/2016</t>
   </si>
   <si>
     <r>
@@ -112,7 +113,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>1</t>
+      <t xml:space="preserve">1</t>
     </r>
     <r>
       <rPr>
@@ -123,7 +124,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>st</t>
+      <t xml:space="preserve">st</t>
     </r>
     <r>
       <rPr>
@@ -133,377 +134,377 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> release</t>
+      <t xml:space="preserve"> release</t>
     </r>
   </si>
   <si>
-    <t>F.Rotenberg</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>This sheet. General information about document usage</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Guidelines on how to used the various sheet</t>
-  </si>
-  <si>
-    <t>IP Release</t>
-  </si>
-  <si>
-    <t>Release information sheet describing</t>
-  </si>
-  <si>
-    <t>IPIF_relx.x</t>
-  </si>
-  <si>
-    <t>IP interface description reference, describing IP symbol/entity and integration and test information relative to IP interface.</t>
-  </si>
-  <si>
-    <t>IPDESCR_Relx.x</t>
-  </si>
-  <si>
-    <t>Description of the main features of the IP</t>
-  </si>
-  <si>
-    <t>IPREGLIST_rely.y</t>
-  </si>
-  <si>
-    <t>Description of the list of registers used by IP. Registers can be physically instanciated inside IP or outside IP.</t>
-  </si>
-  <si>
-    <t>IPREGMAP_relz.z</t>
-  </si>
-  <si>
-    <t>Description of mapping of bit fields when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
-  </si>
-  <si>
-    <t>IPTREGMAP_relz.z</t>
-  </si>
-  <si>
-    <t>Description of mapping of test bit field when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
-  </si>
-  <si>
-    <t>IP Release Sheet</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Possible Value</t>
-  </si>
-  <si>
-    <t>IP release version numeroted as [major release].[minor release]. A release is major whenever IP interface is modified.</t>
-  </si>
-  <si>
-    <t>X.Y. Z</t>
-  </si>
-  <si>
-    <t>Release description</t>
-  </si>
-  <si>
-    <t>This is a free text entry expliciting the release main modifications and purpose.</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>IPIF</t>
-  </si>
-  <si>
-    <t>IPIF sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPDESCR</t>
-  </si>
-  <si>
-    <t>IPDESCR sheet version to nbe used for this release</t>
-  </si>
-  <si>
-    <t>X.Y.Z</t>
-  </si>
-  <si>
-    <t>IPREGLIST</t>
-  </si>
-  <si>
-    <t>IPREGLIST sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPREGMAP</t>
-  </si>
-  <si>
-    <t>IPREGMAP sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPDOC</t>
-  </si>
-  <si>
-    <t>IPDOC version to be used for this release.</t>
-  </si>
-  <si>
-    <t>GIT version</t>
-  </si>
-  <si>
-    <t>GIT database number corresponding to IP design code and IP reference XLS.</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>IPIF sheet</t>
-  </si>
-  <si>
-    <t>IP Interface description</t>
-  </si>
-  <si>
-    <t>IP Pin Name</t>
-  </si>
-  <si>
-    <t>Name of IP Pin. This must must exactly name find in code or schematic (including case).</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>Direction or type of signal</t>
-  </si>
-  <si>
-    <t>In,Out,IO</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Analog, Digital, supply, DR (Dual Rail), SR (SingleRail)</t>
-  </si>
-  <si>
-    <t>Analog,Digital, VDD, GND, DR, SR</t>
-  </si>
-  <si>
-    <t>Voltage Domain</t>
-  </si>
-  <si>
-    <t>Clock domain</t>
-  </si>
-  <si>
-    <t>IO</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Reset Value</t>
-  </si>
-  <si>
-    <t>Integration information</t>
-  </si>
-  <si>
-    <t>Integration comment</t>
-  </si>
-  <si>
-    <t>Core Interface</t>
-  </si>
-  <si>
-    <t>Register  Interface</t>
-  </si>
-  <si>
-    <t>Register name</t>
-  </si>
-  <si>
-    <t>DFT value</t>
-  </si>
-  <si>
-    <t>Level Shifter</t>
-  </si>
-  <si>
-    <t>Isolation cell</t>
-  </si>
-  <si>
-    <t>Connected to</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Destination supply</t>
-  </si>
-  <si>
-    <t>Hard Macro information</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>layer</t>
-  </si>
-  <si>
-    <t>Antenna</t>
-  </si>
-  <si>
-    <t>Additonal Information</t>
-  </si>
-  <si>
-    <t>FreeText 1</t>
-  </si>
-  <si>
-    <t>FreeText 2</t>
-  </si>
-  <si>
-    <t>Driver information</t>
-  </si>
-  <si>
-    <t>Function1</t>
-  </si>
-  <si>
-    <t>Function2</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>Rel1.0.0</t>
-  </si>
-  <si>
-    <t>Bit position</t>
-  </si>
-  <si>
-    <t>Trim during production</t>
-  </si>
-  <si>
-    <t>clk_i</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>digital</t>
-  </si>
-  <si>
-    <t>rstn_i</t>
-  </si>
-  <si>
-    <t>uart_rx_i</t>
-  </si>
-  <si>
-    <t>uart_tx_o</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
-    <t>cfg_data_i</t>
-  </si>
-  <si>
-    <t>cfg_addr_i</t>
-  </si>
-  <si>
-    <t>cfg_valid_i</t>
-  </si>
-  <si>
-    <t>cfg_rwn_i</t>
-  </si>
-  <si>
-    <t>cfg_data_o</t>
-  </si>
-  <si>
-    <t>cfg_ready_o</t>
-  </si>
-  <si>
-    <t>cfg_rx_startaddr_o</t>
-  </si>
-  <si>
-    <t>cfg_rx_size_o</t>
-  </si>
-  <si>
-    <t>cfg_rx_datasize_o</t>
-  </si>
-  <si>
-    <t>cfg_rx_continuous_o</t>
-  </si>
-  <si>
-    <t>cfg_rx_en_o</t>
-  </si>
-  <si>
-    <t>cfg_rx_clr_o</t>
-  </si>
-  <si>
-    <t>cfg_rx_en_i</t>
-  </si>
-  <si>
-    <t>cfg_rx_pending_i</t>
-  </si>
-  <si>
-    <t>cfg_rx_curr_addr_i</t>
-  </si>
-  <si>
-    <t>cfg_rx_bytes_left_i</t>
-  </si>
-  <si>
-    <t>cfg_tx_startaddr_o</t>
-  </si>
-  <si>
-    <t>cfg_tx_size_o</t>
-  </si>
-  <si>
-    <t>cfg_tx_datasize_o</t>
-  </si>
-  <si>
-    <t>cfg_tx_continuous_o</t>
-  </si>
-  <si>
-    <t>cfg_tx_en_o</t>
-  </si>
-  <si>
-    <t>cfg_tx_clr_o</t>
-  </si>
-  <si>
-    <t>cfg_tx_en_i</t>
-  </si>
-  <si>
-    <t>cfg_tx_pending_i</t>
-  </si>
-  <si>
-    <t>cfg_tx_curr_addr_i</t>
-  </si>
-  <si>
-    <t>cfg_tx_bytes_left_i</t>
-  </si>
-  <si>
-    <t>data_rx_datasize_o</t>
-  </si>
-  <si>
-    <t>data_rx_data_o</t>
-  </si>
-  <si>
-    <t>data_rx_valid_o</t>
-  </si>
-  <si>
-    <t>data_rx_ready_i</t>
-  </si>
-  <si>
-    <t>data_tx_datasize_o</t>
-  </si>
-  <si>
-    <t>data_tx_data_i</t>
-  </si>
-  <si>
-    <t>data_tx_valid_i</t>
-  </si>
-  <si>
-    <t>data_tx_ready_o</t>
-  </si>
-  <si>
-    <t>UART component manages the following features:
+    <t xml:space="preserve">F.Rotenberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sheet. General information about document usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guidelines on how to used the various sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release information sheet describing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF_relx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP interface description reference, describing IP symbol/entity and integration and test information relative to IP interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR_Relx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the main features of the IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST_rely.y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the list of registers used by IP. Registers can be physically instanciated inside IP or outside IP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of mapping of bit fields when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPTREGMAP_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of mapping of test bit field when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Release Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possible Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP release version numeroted as [major release].[minor release]. A release is major whenever IP interface is modified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X.Y. Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a free text entry expliciting the release main modifications and purpose.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR sheet version to nbe used for this release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X.Y.Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDOC version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT database number corresponding to IP design code and IP reference XLS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Interface description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Pin Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of IP Pin. This must must exactly name find in code or schematic (including case).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction or type of signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In,Out,IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog, Digital, supply, DR (Dual Rail), SR (SingleRail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog,Digital, VDD, GND, DR, SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage Domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register  Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFT value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Shifter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isolation cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connected to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard Macro information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additonal Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeText 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeText 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trim during production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rstn_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uart_rx_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uart_tx_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_data_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_addr_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_valid_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rwn_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_data_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_ready_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_startaddr_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_size_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_datasize_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_continuous_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_en_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_clr_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_en_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_pending_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_curr_addr_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_rx_bytes_left_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_startaddr_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_size_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_datasize_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_continuous_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_en_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_clr_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_en_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_pending_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_curr_addr_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_tx_bytes_left_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_rx_datasize_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_rx_data_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_rx_valid_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_rx_ready_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_tx_datasize_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_tx_data_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_tx_valid_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_tx_ready_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART component manages the following features:
 - Standard full-duplex UART interface
 - Configurable baudrate related to SoC domain clock frequency
 - Configurable parity bit generation and check
@@ -511,275 +512,401 @@
 - Configurable character length</t>
   </si>
   <si>
-    <t>Register Name</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Register Type</t>
-  </si>
-  <si>
-    <t>Host Access Type</t>
-  </si>
-  <si>
-    <t>IP access Type</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>FootNote</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>RX_SADDR</t>
-  </si>
-  <si>
-    <t>0x0</t>
-  </si>
-  <si>
-    <t>Config</t>
-  </si>
-  <si>
-    <t>R/W</t>
-  </si>
-  <si>
-    <t>uDMA RX UART buffer base address configuration register.</t>
-  </si>
-  <si>
-    <t>RX_SIZE</t>
-  </si>
-  <si>
-    <t>0x4</t>
-  </si>
-  <si>
-    <t>uDMA RX UART buffer size configuration register.</t>
-  </si>
-  <si>
-    <t>RX_CFG</t>
-  </si>
-  <si>
-    <t>0x8</t>
-  </si>
-  <si>
-    <t>uDMA RX UART stream configuration register.</t>
-  </si>
-  <si>
-    <t>TX_SADDR</t>
-  </si>
-  <si>
-    <t>0x10</t>
-  </si>
-  <si>
-    <t>uDMA TX UART buffer base address configuration register.</t>
-  </si>
-  <si>
-    <t>TX_SIZE</t>
-  </si>
-  <si>
-    <t>0x14</t>
-  </si>
-  <si>
-    <t>uDMA TX UART buffer size configuration register.</t>
-  </si>
-  <si>
-    <t>TX_CFG</t>
-  </si>
-  <si>
-    <t>0x18</t>
-  </si>
-  <si>
-    <t>uDMA TX UART stream configuration register.</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>0x20</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>uDMA UART status register.</t>
-  </si>
-  <si>
-    <t>SETUP</t>
-  </si>
-  <si>
-    <t>0x24</t>
-  </si>
-  <si>
-    <t>UDMA UART configuration register.</t>
-  </si>
-  <si>
-    <t>Bit field</t>
-  </si>
-  <si>
-    <t>Register</t>
-  </si>
-  <si>
-    <t>Bit Position</t>
-  </si>
-  <si>
-    <t>RX buffer base address bitfield:
+    <t xml:space="preserve">Register Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host Access Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP access Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FootNote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX_SADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R/W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA RX UART buffer base address configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX_SIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA RX UART buffer size configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX_CFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA RX UART stream configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX_SADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA TX UART buffer base address configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX_SIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA TX UART buffer size configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX_CFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA TX UART stream configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA UART status register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SETUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDMA UART configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX buffer base address bitfield:
 - Read: returns value of the buffer pointer until transfer is finished. Else returns 0.
 - Write: sets RX buffer base address</t>
   </si>
   <si>
-    <t>RX buffer size bitfield in bytes. (128kBytes maximum)
+    <t xml:space="preserve">RX buffer size bitfield in bytes. (128kBytes maximum)
 - Read: returns remaining buffer size to transfer.
 - Write: sets buffer size.</t>
   </si>
   <si>
-    <t>CONTINOUS</t>
-  </si>
-  <si>
-    <t>RX channel continuous mode bitfield:
+    <t xml:space="preserve">CONTINOUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX channel continuous mode bitfield:
 -1'b0: disabled
 -1'b1: enabled
 At the end of the buffer transfer, the uDMA reloads the address / buffer size and starts a new transfer.</t>
   </si>
   <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t>RX channel enable and start transfer bitfield:
+    <t xml:space="preserve">EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX channel enable and start transfer bitfield:
 -1'b0: disable
 -1'b1: enable and start the transfer
 This signal is used also to queue a transfer if one is already ongoing.</t>
   </si>
   <si>
-    <t>CLR</t>
-  </si>
-  <si>
-    <t>RX channel clear and stop transfer:
+    <t xml:space="preserve">CLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX channel clear and stop transfer:
 -1'b0: disable
 -1'b1: stop and clear the on-going transfer</t>
   </si>
   <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>RX transfer pending in queue status flag:
+    <t xml:space="preserve">PENDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX transfer pending in queue status flag:
 -1'b0: no pending transfer in the queue
 -1'b1: pending transfer in the queue</t>
   </si>
   <si>
-    <t>TX buffer base address bitfield:
+    <t xml:space="preserve">TX buffer base address bitfield:
 - Read: returns value of the buffer pointer until transfer is finished. Else returns 0.
 - Write: sets buffer base address</t>
   </si>
   <si>
-    <t>TX buffer size bitfield in bytes. (128kBytes maximum)
+    <t xml:space="preserve">TX buffer size bitfield in bytes. (128kBytes maximum)
 - Read: returns remaining buffer size to transfer.
 - Write: sets buffer size.</t>
   </si>
   <si>
-    <t>TX channel continuous mode bitfield:
+    <t xml:space="preserve">TX channel continuous mode bitfield:
 -1'b0: disabled
 -1'b1: enabled
 At the end of the buffer transfer, the uDMA reloads the address / buffer size and starts a new transfer.</t>
   </si>
   <si>
-    <t>TX channel enable and start transfer bitfield:
+    <t xml:space="preserve">TX channel enable and start transfer bitfield:
 -1'b0: disabled
 -1'b1: enable and start the transfer
 This signal is used also to queue a transfer if one is already ongoing.</t>
   </si>
   <si>
-    <t>TX channel clear and stop transfer bitfield:
+    <t xml:space="preserve">TX channel clear and stop transfer bitfield:
 -1'b0: disabled
 -1'b1: stop and clear the on-going transfer</t>
   </si>
   <si>
-    <t>TX transfer pending in queue status flag:
+    <t xml:space="preserve">TX transfer pending in queue status flag:
 -1'b0: no pending transfer in the queue
 -1'b1: pending transfer in the queue</t>
   </si>
   <si>
-    <t>TX_BUSY</t>
-  </si>
-  <si>
-    <t>TX busy status flag:
+    <t xml:space="preserve">TX_BUSY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX busy status flag:
 - 1'b0: no TX transfer on-going
 - 1'b1: TX transfer on-going</t>
   </si>
   <si>
-    <t>RX_BUSY</t>
-  </si>
-  <si>
-    <t>RX busy status flag:
+    <t xml:space="preserve">RX_BUSY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX busy status flag:
 - 1'b0: no RX transfer on-going
 - 1'b1: RX transfer on-going</t>
   </si>
   <si>
-    <t>RX_PE</t>
-  </si>
-  <si>
-    <t>RX parity error status flag:
+    <t xml:space="preserve">RX_PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX parity error status flag:
 - 1'b0: no error
 - 1'b1: RX parity error occurred </t>
   </si>
   <si>
-    <t>PARITY_ENA</t>
-  </si>
-  <si>
-    <t>Parity bit generation and check configuration bitfield:
+    <t xml:space="preserve">PARITY_ENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parity bit generation and check configuration bitfield:
 - 1'b0: disabled
 - 1'b1: enabled</t>
   </si>
   <si>
-    <t>BIT_LENGTH</t>
-  </si>
-  <si>
-    <t>Character length bitfield:
+    <t xml:space="preserve">BIT_LENGTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Character length bitfield:
 - 2'b00: 5 bits
 - 2'b01: 6 bits
 - 2'b10: 7 bits
 - 2'b11: 8 bits</t>
   </si>
   <si>
-    <t>STOP_BITS</t>
-  </si>
-  <si>
-    <t>Stop bits length bitfield:
+    <t xml:space="preserve">STOP_BITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop bits length bitfield:
 - 1'b0: 1 stop bit
 - 1'b1: 2 stop bits</t>
   </si>
   <si>
-    <t>TX_ENA</t>
-  </si>
-  <si>
-    <t>TX transceiver configuration bitfield:
+    <t xml:space="preserve">TX_ENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX transceiver configuration bitfield:
 - 1'b0: disabled
 - 1'b1: enabled</t>
   </si>
   <si>
-    <t>RX_ENA</t>
-  </si>
-  <si>
-    <t>RX transceiver configuration bitfield:
+    <t xml:space="preserve">RX_ENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX transceiver configuration bitfield:
 - 1'b0: disabled
 - 1'b1: enabled</t>
   </si>
   <si>
-    <t>CLKDIV</t>
-  </si>
-  <si>
-    <t>UART Clock divider configuration bitfield. The baudrate is equal to SOC_FREQ/CLKDIV.</t>
-  </si>
-  <si>
-    <t>testcase location&amp;name</t>
+    <t xml:space="preserve">CLKDIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART Clock divider configuration bitfield. The baudrate is equal to SOC_FREQ/CLKDIV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDMA_GC-&gt;CG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1A102000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOCEU-&gt;FC_MASK[8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1A106004 – 0x1A106024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Start/Stop IP clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear UDMA clock gating register bit 4 for UART0 or bit 5 for UART1 = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP has the clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set UDMA clock gating register bit 4 for UART0 or bit 5 for UART1 = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP has no clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Enable or disable IP interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear SoC event unit FC interrupt mask UART’s events’ index  = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP’s interrupt can go to microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set SoC event unit FC interrupt mask UART’s events’ index  = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP’s interrupt can not go to microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Frequency control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set CLKDIV  to the number wanted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP’s frequency = Perpheral frequency / (CLKDIV*2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must after operation 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. UART RX TX enable control </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set  TX_ENA = 1 and RX_ENA = 1 to enable RX and TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP enable RX TX according to setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Format control </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set  PARITY_ENA, BIT_LENGTH, STOP_BITS to the right value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP sets format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must after operation 1, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Send data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocation L2 tranfer buffer
+Set SETUP TX_ENA = 1
+Set TX_SADDR = buffer start pointer address
+Set TX_SIZE       =  buffer size
+Set TX_CFG  register EN bit = 1  
+Wait IP transfer finished (IRQ)
+Check STATUS to see if there is error or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+IP start to transfer data, busy
+TX_CFG  register EN bit = 0 , Transfer finished
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must after operation 2, 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Receive data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocation L2 tranfer buffer
+Set  SETUP RX_ENA = 1
+Set RX_SADDR = buffer start pointer address
+Set RX_SIZE       =  buffer size
+Set RX_CFG  register EN bit = 1  
+Wait IP transfer finished (IRQ)
+Check STATUS to see if there is error or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+IP start to transfer data, busy
+RX_CFG  register EN bit = 0 , Transfer finished
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testcase location&amp;name</t>
   </si>
 </sst>
 </file>
@@ -787,9 +914,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -837,6 +964,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1006,7 +1141,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1257,6 +1392,14 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1343,16 +1486,16 @@
   </sheetPr>
   <dimension ref="B3:D29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,7 +1698,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1570,16 +1713,17 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6173469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +2038,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1909,14 +2053,17 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.1632653061224"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,7 +2112,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1980,21 +2127,21 @@
   </sheetPr>
   <dimension ref="A1:AC40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2581,7 +2728,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2596,14 +2743,14 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="193.84693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="50" width="191.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,7 +2766,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2632,25 +2779,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K65536"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="true" max="2" min="2" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="51.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,7 +3055,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2921,25 +3068,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.1632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="72.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3554,7 +3701,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3567,38 +3714,232 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A3:D21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.34"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="63"/>
+      <c r="D6" s="40"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="64" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="58"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+    </row>
+    <row r="20" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="58" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>249</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="58" t="s">
+        <v>252</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="63" t="s">
-        <v>219</v>
-      </c>
-      <c r="D1" s="63" t="s">
+      <c r="C1" s="65" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="65" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Improved error management and added RX character event
</commit_message>
<xml_diff>
--- a/docs/UART_reference.xlsx
+++ b/docs/UART_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="263">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -504,6 +504,12 @@
     <t xml:space="preserve">data_tx_ready_o</t>
   </si>
   <si>
+    <t xml:space="preserve">rx_char_event_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">err_event_o</t>
+  </si>
+  <si>
     <t xml:space="preserve">UART component manages the following features:
 - Standard full-duplex UART interface
 - Configurable baudrate related to SoC domain clock frequency
@@ -623,6 +629,15 @@
     <t xml:space="preserve">UDMA UART configuration register.</t>
   </si>
   <si>
+    <t xml:space="preserve">ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA UART Error status</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bit field</t>
   </si>
   <si>
@@ -722,14 +737,6 @@
     <t xml:space="preserve">RX busy status flag:
 - 1'b0: no RX transfer on-going
 - 1'b1: RX transfer on-going</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX_PE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX parity error status flag:
-- 1'b0: no error
-- 1'b1: RX parity error occurred </t>
   </si>
   <si>
     <t xml:space="preserve">PARITY_ENA</t>
@@ -778,6 +785,22 @@
   </si>
   <si>
     <t xml:space="preserve">UART Clock divider configuration bitfield. The baudrate is equal to SOC_FREQ/CLKDIV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX_ERR_OVERFLOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX overflow error status flag:
+- 1'b0: no error
+- 1'b1: RX overflow error occurred </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX_ERR_PARITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX parity error status flag:
+- 1'b0: no error
+- 1'b1: RX parity error occurred </t>
   </si>
   <si>
     <t xml:space="preserve">UDMA_GC-&gt;CG</t>
@@ -1486,16 +1509,16 @@
   </sheetPr>
   <dimension ref="B3:D29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,7 +1721,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1713,17 +1736,17 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,7 +2061,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2053,17 +2076,17 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,7 +2135,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2125,23 +2148,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC40"/>
+  <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="21" min="16" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,6 +2712,28 @@
         <v>109</v>
       </c>
       <c r="C40" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="41" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2728,7 +2773,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2743,14 +2788,14 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="50" width="191.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.39"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="189.663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2760,13 +2805,13 @@
     </row>
     <row r="2" customFormat="false" ht="96.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2779,224 +2824,224 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="51.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="true" max="2" min="2" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.1632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="53" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D1" s="53" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I1" s="54" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="K1" s="53" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="55" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D2" s="55" t="n">
         <v>32</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F2" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="G2" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>155</v>
-      </c>
       <c r="I2" s="52" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D3" s="55" t="n">
         <v>32</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F3" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="G3" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" s="56" t="s">
-        <v>155</v>
-      </c>
       <c r="I3" s="52" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="55" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D4" s="55" t="n">
         <v>32</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F4" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="H4" s="56" t="s">
-        <v>155</v>
-      </c>
       <c r="I4" s="52" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="55" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D5" s="55" t="n">
         <v>32</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F5" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="H5" s="56" t="s">
-        <v>155</v>
-      </c>
       <c r="I5" s="52" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="55" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D6" s="55" t="n">
         <v>32</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F6" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>155</v>
-      </c>
       <c r="I6" s="52" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="55" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D7" s="55" t="n">
         <v>32</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F7" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="H7" s="56" t="s">
-        <v>155</v>
-      </c>
       <c r="I7" s="52" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="55" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D8" s="55" t="n">
         <v>32</v>
@@ -3005,43 +3050,69 @@
         <v>9</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H8" s="56" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J8" s="56"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="55" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D9" s="55" t="n">
         <v>32</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F9" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="H9" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="G9" s="56" t="s">
-        <v>176</v>
-      </c>
-      <c r="H9" s="56" t="s">
-        <v>155</v>
-      </c>
       <c r="I9" s="52" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3055,7 +3126,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3068,45 +3139,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="72.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="71.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G1" s="40" t="s">
         <v>76</v>
@@ -3117,10 +3188,10 @@
     </row>
     <row r="2" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="58" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C2" s="50" t="n">
         <v>0</v>
@@ -3129,24 +3200,24 @@
         <v>16</v>
       </c>
       <c r="E2" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H2" s="60" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="58" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C3" s="50" t="n">
         <v>0</v>
@@ -3155,24 +3226,24 @@
         <v>17</v>
       </c>
       <c r="E3" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H3" s="60" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="58" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C4" s="50" t="n">
         <v>0</v>
@@ -3181,24 +3252,24 @@
         <v>1</v>
       </c>
       <c r="E4" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F4" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H4" s="60" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="58" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C5" s="50" t="n">
         <v>4</v>
@@ -3207,24 +3278,24 @@
         <v>1</v>
       </c>
       <c r="E5" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H5" s="60" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="58" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C6" s="50" t="n">
         <v>5</v>
@@ -3233,24 +3304,24 @@
         <v>1</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="58" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C7" s="50" t="n">
         <v>5</v>
@@ -3259,24 +3330,24 @@
         <v>1</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H7" s="60" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="58" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C8" s="50" t="n">
         <v>0</v>
@@ -3285,24 +3356,24 @@
         <v>16</v>
       </c>
       <c r="E8" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G8" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H8" s="60" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="58" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C9" s="50" t="n">
         <v>0</v>
@@ -3311,24 +3382,24 @@
         <v>17</v>
       </c>
       <c r="E9" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G9" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H9" s="60" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="58" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C10" s="50" t="n">
         <v>0</v>
@@ -3337,24 +3408,24 @@
         <v>1</v>
       </c>
       <c r="E10" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H10" s="60" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="58" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C11" s="50" t="n">
         <v>4</v>
@@ -3363,24 +3434,24 @@
         <v>1</v>
       </c>
       <c r="E11" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="59" t="s">
-        <v>155</v>
-      </c>
       <c r="H11" s="60" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="58" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C12" s="50" t="n">
         <v>5</v>
@@ -3389,24 +3460,24 @@
         <v>1</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G12" s="59" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H12" s="60" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="58" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C13" s="50" t="n">
         <v>5</v>
@@ -3415,24 +3486,24 @@
         <v>1</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F13" s="50" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H13" s="60" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="58" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C14" s="41" t="n">
         <v>0</v>
@@ -3441,24 +3512,24 @@
         <v>1</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F14" s="59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H14" s="60" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="58" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C15" s="41" t="n">
         <v>1</v>
@@ -3467,50 +3538,25 @@
         <v>1</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F15" s="59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H15" s="60" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="58" t="s">
-        <v>205</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>174</v>
-      </c>
-      <c r="C16" s="41" t="n">
-        <v>2</v>
-      </c>
-      <c r="D16" s="41" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="F16" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="H16" s="60" t="s">
-        <v>206</v>
-      </c>
-    </row>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="58" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C17" s="41" t="n">
         <v>0</v>
@@ -3519,24 +3565,24 @@
         <v>1</v>
       </c>
       <c r="E17" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="G17" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="F17" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>155</v>
-      </c>
       <c r="H17" s="60" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="58" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C18" s="41" t="n">
         <v>1</v>
@@ -3545,24 +3591,24 @@
         <v>2</v>
       </c>
       <c r="E18" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="G18" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>155</v>
-      </c>
       <c r="H18" s="60" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="58" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C19" s="41" t="n">
         <v>3</v>
@@ -3571,24 +3617,24 @@
         <v>1</v>
       </c>
       <c r="E19" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>155</v>
-      </c>
       <c r="H19" s="60" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="58" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C20" s="41" t="n">
         <v>8</v>
@@ -3597,24 +3643,24 @@
         <v>1</v>
       </c>
       <c r="E20" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F20" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="G20" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="F20" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>155</v>
-      </c>
       <c r="H20" s="60" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="58" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B21" s="56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C21" s="41" t="n">
         <v>9</v>
@@ -3623,24 +3669,24 @@
         <v>1</v>
       </c>
       <c r="E21" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="F21" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>155</v>
-      </c>
       <c r="H21" s="60" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="58" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B22" s="56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C22" s="41" t="n">
         <v>16</v>
@@ -3649,35 +3695,69 @@
         <v>16</v>
       </c>
       <c r="E22" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="F22" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>155</v>
-      </c>
       <c r="H22" s="60" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="56"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="61"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="56"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="61"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C23" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="60" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="41"/>
@@ -3701,7 +3781,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3716,37 +3796,38 @@
   </sheetPr>
   <dimension ref="A3:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.34"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B6" s="63" t="s">
         <v>11</v>
@@ -3756,65 +3837,65 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="64" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="58" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C14" s="58" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,16 +3905,16 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="58" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,16 +3924,16 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="58" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3862,30 +3943,30 @@
     </row>
     <row r="20" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="58" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="58" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3894,7 +3975,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3909,17 +3990,17 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3930,7 +4011,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D1" s="65" t="s">
         <v>9</v>
@@ -3939,7 +4020,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Improve uart by adding RX IRQ and polling method
</commit_message>
<xml_diff>
--- a/docs/UART_reference.xlsx
+++ b/docs/UART_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="282">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -638,6 +638,36 @@
     <t xml:space="preserve">uDMA UART Error status</t>
   </si>
   <si>
+    <t xml:space="preserve">IRQ_EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA UART Read or Error interrupt enable register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA UART Read polling data valid flag register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA UART Read polling data register.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bit field</t>
   </si>
   <si>
@@ -765,6 +795,14 @@
 - 1'b1: 2 stop bits</t>
   </si>
   <si>
+    <t xml:space="preserve">POLLING_EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When in uart read, use polling method to read the data,  read interrupt enable flag will be ignored:
+- 1'b0: Do not using polling method to read data.
+- 1'b1: Using polling method to read data. Interrupt enable flag will be ignored.</t>
+  </si>
+  <si>
     <t xml:space="preserve">TX_ENA</t>
   </si>
   <si>
@@ -801,6 +839,33 @@
     <t xml:space="preserve">RX parity error status flag:
 - 1'b0: no error
 - 1'b1: RX parity error occurred </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rx interrupt in enable flag:
+- 1'b0: RX IRQ disable
+- 1'b1: RX IRQ enable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error interrupt in enable flag:
+- 1'b0: Error IRQ disable
+- 1'b1: Error IRQ enable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">READY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used only in RX polling method to indicate data is ready for read:
+- 1'b0: Data is not ready to read
+- 1'b1: Data is ready to read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX read data for polling or interrupt</t>
   </si>
   <si>
     <t xml:space="preserve">UDMA_GC-&gt;CG</t>
@@ -939,7 +1004,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -986,13 +1051,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1011,7 +1069,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF77933C"/>
-        <bgColor rgb="FF76923C"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -1027,7 +1085,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1119,21 +1177,6 @@
       <bottom style="thick"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thick">
-        <color rgb="FF76923C"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF77933C"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF77933C"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF77933C"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1164,7 +1207,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1409,19 +1452,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1452,11 +1487,11 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF76923C"/>
+      <rgbColor rgb="FF77933C"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC3D69B"/>
-      <rgbColor rgb="FF77933C"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1515,10 +1550,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,11 +1775,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2076,17 +2109,17 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,15 +2189,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,8 +2823,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="189.663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="187.637755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,20 +2858,16 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
     <col collapsed="false" hidden="true" max="2" min="2" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.1632653061225"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="50.484693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3113,6 +3138,84 @@
       </c>
       <c r="I10" s="0" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3139,36 +3242,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="71.5459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>75</v>
@@ -3209,7 +3310,7 @@
         <v>157</v>
       </c>
       <c r="H2" s="60" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,12 +3336,12 @@
         <v>157</v>
       </c>
       <c r="H3" s="60" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="58" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B4" s="56" t="s">
         <v>164</v>
@@ -3261,12 +3362,12 @@
         <v>157</v>
       </c>
       <c r="H4" s="60" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="58" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="B5" s="56" t="s">
         <v>164</v>
@@ -3287,12 +3388,12 @@
         <v>157</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="58" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B6" s="56" t="s">
         <v>164</v>
@@ -3313,12 +3414,12 @@
         <v>157</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="58" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B7" s="56" t="s">
         <v>164</v>
@@ -3339,7 +3440,7 @@
         <v>157</v>
       </c>
       <c r="H7" s="60" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,7 +3466,7 @@
         <v>157</v>
       </c>
       <c r="H8" s="60" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3391,12 +3492,12 @@
         <v>157</v>
       </c>
       <c r="H9" s="60" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="58" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B10" s="56" t="s">
         <v>173</v>
@@ -3417,12 +3518,12 @@
         <v>157</v>
       </c>
       <c r="H10" s="60" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="58" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="B11" s="56" t="s">
         <v>173</v>
@@ -3443,12 +3544,12 @@
         <v>157</v>
       </c>
       <c r="H11" s="60" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="58" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B12" s="56" t="s">
         <v>173</v>
@@ -3469,12 +3570,12 @@
         <v>157</v>
       </c>
       <c r="H12" s="60" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="58" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B13" s="56" t="s">
         <v>173</v>
@@ -3495,12 +3596,12 @@
         <v>157</v>
       </c>
       <c r="H13" s="60" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="58" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="B14" s="56" t="s">
         <v>176</v>
@@ -3521,12 +3622,12 @@
         <v>157</v>
       </c>
       <c r="H14" s="60" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="58" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B15" s="56" t="s">
         <v>176</v>
@@ -3547,13 +3648,12 @@
         <v>157</v>
       </c>
       <c r="H15" s="60" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>219</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="58" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B17" s="56" t="s">
         <v>181</v>
@@ -3574,12 +3674,12 @@
         <v>157</v>
       </c>
       <c r="H17" s="60" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="58" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B18" s="56" t="s">
         <v>181</v>
@@ -3600,12 +3700,12 @@
         <v>157</v>
       </c>
       <c r="H18" s="60" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="58" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B19" s="56" t="s">
         <v>181</v>
@@ -3626,20 +3726,20 @@
         <v>157</v>
       </c>
       <c r="H19" s="60" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="58" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B20" s="56" t="s">
         <v>181</v>
       </c>
       <c r="C20" s="41" t="n">
-        <v>8</v>
-      </c>
-      <c r="D20" s="41" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="59" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="59" t="s">
@@ -3652,18 +3752,18 @@
         <v>157</v>
       </c>
       <c r="H20" s="60" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="58" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="B21" s="56" t="s">
         <v>181</v>
       </c>
       <c r="C21" s="41" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="41" t="n">
         <v>1</v>
@@ -3678,21 +3778,21 @@
         <v>157</v>
       </c>
       <c r="H21" s="60" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="58" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B22" s="56" t="s">
         <v>181</v>
       </c>
       <c r="C22" s="41" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D22" s="41" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E22" s="59" t="s">
         <v>159</v>
@@ -3704,44 +3804,44 @@
         <v>157</v>
       </c>
       <c r="H22" s="60" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="58" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="B23" s="56" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C23" s="41" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D23" s="41" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E23" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" s="59" t="s">
         <v>178</v>
-      </c>
-      <c r="F23" s="59" t="s">
-        <v>179</v>
       </c>
       <c r="G23" s="41" t="s">
         <v>157</v>
       </c>
       <c r="H23" s="60" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="58" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="B24" s="56" t="s">
         <v>184</v>
       </c>
       <c r="C24" s="41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="41" t="n">
         <v>1</v>
@@ -3756,28 +3856,139 @@
         <v>157</v>
       </c>
       <c r="H24" s="60" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="61"/>
-    </row>
-    <row r="26" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="50"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="62"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F25" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="G25" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="B26" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" s="60" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="41.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="60" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H28" s="60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="50" t="n">
+        <v>8</v>
+      </c>
+      <c r="E29" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F29" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3802,100 +4013,100 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>230</v>
-      </c>
-      <c r="B6" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="63"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="40"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="64" t="s">
-        <v>231</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>232</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>233</v>
+      <c r="B7" s="62" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="58" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="C14" s="58" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,16 +4116,16 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="58" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,16 +4135,16 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="58" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3943,30 +4154,30 @@
     </row>
     <row r="20" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="58" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="58" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3997,23 +4208,23 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="65" t="s">
-        <v>262</v>
-      </c>
-      <c r="D1" s="65" t="s">
+      <c r="C1" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="63" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>